<commit_message>
Relleno sin remocion outlier
</commit_message>
<xml_diff>
--- a/Hydrology/Validación Maipo/NSE_v3_4.xlsx
+++ b/Hydrology/Validación Maipo/NSE_v3_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccalvo\Documents\GitHub\WEAP-MODFLOW-personal\Hydrology\Validación Maipo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E11699-3F95-4C76-8109-689B9881BC33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B370D3EA-D86F-436A-9655-9CB977B135A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{44936DEA-F884-4270-BD19-0D66D5FA4EA8}"/>
   </bookViews>
@@ -237,7 +237,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -271,7 +271,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4232,15 +4232,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70575A4B-5B9E-41A5-9EEE-8A3E9FA0C948}">
-  <dimension ref="B1:W19"/>
+  <dimension ref="B1:X19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>19</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -4339,8 +4339,11 @@
       <c r="W2">
         <v>0.90333847660088595</v>
       </c>
+      <c r="X2">
+        <v>0.916911241968002</v>
+      </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -4366,7 +4369,7 @@
         <v>0.93740570122244504</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -4392,7 +4395,7 @@
         <v>0.96380145431171504</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -4418,7 +4421,7 @@
         <v>0.97592358982849903</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -4444,7 +4447,7 @@
         <v>0.96721907556961795</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -4470,7 +4473,7 @@
         <v>0.91203085332078504</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -4496,7 +4499,7 @@
         <v>0.79191090720385504</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -4522,7 +4525,7 @@
         <v>0.97827427948569401</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -4548,7 +4551,7 @@
         <v>0.96251782471001102</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -4574,7 +4577,7 @@
         <v>0.98885216350385796</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -4600,7 +4603,7 @@
         <v>0.986545359170799</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -4626,7 +4629,7 @@
         <v>0.88294244248971798</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -4652,7 +4655,7 @@
         <v>0.80486596783708597</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -4678,7 +4681,7 @@
         <v>0.96040581667745795</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>16</v>
       </c>

</xml_diff>